<commit_message>
Stalagmite not stalagnite, and updted game mechanics in tarefas
</commit_message>
<xml_diff>
--- a/grupo_1_macro_gd1_2022_2023.xlsx
+++ b/grupo_1_macro_gd1_2022_2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grupolusofona-my.sharepoint.com/personal/a22204782_alunos_ulht_pt/Documents/Desktop/fcul/GD1/pedro/TP2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e04e61c3d21d2551/Ambiente de Trabalho/GD2/GD2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{7BCFC019-B8E2-4345-9B90-948E82B26FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E2BCF4B-042B-45FD-813D-42A91532859C}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{7BCFC019-B8E2-4345-9B90-948E82B26FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32DC5DA1-D22E-4CC3-92EA-4F7A9E2CC0E8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game Design Macro" sheetId="2" r:id="rId1"/>
@@ -232,9 +232,6 @@
     <t>Take a breather as you jump to the next area</t>
   </si>
   <si>
-    <t>• Charged Jump, Stalagnite Throw</t>
-  </si>
-  <si>
     <t>•Shoot a stalagnite at the bridge's rope and get to the next area</t>
   </si>
   <si>
@@ -308,9 +305,6 @@
     <t>The player falls down a big gap from the cloudy edges into na extremely dark cavern</t>
   </si>
   <si>
-    <t>Charged Jump, Stalagnite Throw, Rope Climb</t>
-  </si>
-  <si>
     <t>•Get out from the darkness</t>
   </si>
   <si>
@@ -365,10 +359,16 @@
     <t>tbd</t>
   </si>
   <si>
-    <t>• Charged Jump, Stalagnite Throw, Rope Climb</t>
+    <t>•Throw the rope to make it over the gap that brought you down</t>
   </si>
   <si>
-    <t>•Throw the rope to make it over the gap that brought you down</t>
+    <t>• Charged Jump, Stalagmite Throw</t>
+  </si>
+  <si>
+    <t>Charged Jump, Stalagmite Throw, Rope Climb</t>
+  </si>
+  <si>
+    <t>• Charged Jump, Stalagmite Throw, Rope Climb</t>
   </si>
 </sst>
 </file>
@@ -766,10 +766,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1072,9 +1068,9 @@
   </sheetPr>
   <dimension ref="A1:J1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1118,7 +1114,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="39" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J1" s="39" t="s">
         <v>7</v>
@@ -1141,16 +1137,16 @@
         <v>12</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>26</v>
@@ -1173,16 +1169,16 @@
         <v>16</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>30</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>17</v>
@@ -1190,10 +1186,10 @@
     </row>
     <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>27</v>
@@ -1202,22 +1198,22 @@
         <v>28</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.25">
@@ -1237,16 +1233,16 @@
         <v>16</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>17</v>
@@ -1266,7 +1262,7 @@
         <v>51</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>58</v>
@@ -1278,13 +1274,13 @@
         <v>52</v>
       </c>
       <c r="I6" s="32" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>32</v>
       </c>
@@ -1298,10 +1294,10 @@
         <v>56</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>59</v>
@@ -1310,7 +1306,7 @@
         <v>60</v>
       </c>
       <c r="I7" s="33" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>41</v>
@@ -1339,10 +1335,10 @@
         <v>65</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I8" s="35" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>42</v>
@@ -1356,25 +1352,25 @@
         <v>66</v>
       </c>
       <c r="C9" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="E9" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="14" t="s">
+      <c r="G9" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="H9" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="H9" s="13" t="s">
-        <v>71</v>
-      </c>
       <c r="I9" s="14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J9" s="13" t="s">
         <v>43</v>
@@ -1385,28 +1381,28 @@
         <v>35</v>
       </c>
       <c r="B10" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>73</v>
-      </c>
       <c r="E10" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="F10" s="16" t="s">
-        <v>78</v>
-      </c>
       <c r="G10" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="H10" s="16" t="s">
-        <v>81</v>
-      </c>
       <c r="I10" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J10" s="17" t="s">
         <v>45</v>
@@ -1417,28 +1413,28 @@
         <v>36</v>
       </c>
       <c r="B11" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>90</v>
-      </c>
       <c r="E11" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G11" s="19" t="s">
         <v>59</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I11" s="36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J11" s="19" t="s">
         <v>48</v>
@@ -1449,28 +1445,28 @@
         <v>37</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I12" s="37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J12" s="21" t="s">
         <v>47</v>
@@ -1481,28 +1477,28 @@
         <v>38</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I13" s="35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J13" s="23" t="s">
         <v>44</v>
@@ -1513,60 +1509,60 @@
         <v>35</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J14" s="17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>106</v>
-      </c>
       <c r="D15" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I15" s="38" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>46</v>
@@ -1583,10 +1579,10 @@
         <v>10</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F16" s="30" t="s">
         <v>20</v>
@@ -1596,7 +1592,7 @@
         <v>23</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J16" s="27" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
finalizei tarefas, fiz pdfs para alguns ficheiros
</commit_message>
<xml_diff>
--- a/grupo_1_macro_gd1_2022_2023.xlsx
+++ b/grupo_1_macro_gd1_2022_2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e04e61c3d21d2551/Ambiente de Trabalho/GD2/GD2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grupolusofona-my.sharepoint.com/personal/a22204782_alunos_ulht_pt/Documents/Desktop/fcul/GD1/pedro/TP2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{7BCFC019-B8E2-4345-9B90-948E82B26FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32DC5DA1-D22E-4CC3-92EA-4F7A9E2CC0E8}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{7BCFC019-B8E2-4345-9B90-948E82B26FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F478D59-9A29-4571-8761-8347070FED5D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game Design Macro" sheetId="2" r:id="rId1"/>
@@ -1069,19 +1069,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.88671875" style="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" style="31" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.33203125" style="31" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.21875" style="31"/>
     <col min="6" max="6" width="23.6640625" style="31" bestFit="1" customWidth="1"/>
@@ -1540,7 +1541,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>39</v>
       </c>
@@ -12438,7 +12439,7 @@
       <c r="I1002" s="29"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>